<commit_message>
Completed Addressing Guided Question Set for Module 2, other than question 7. Addressed some personal questions relating to R.
Going to study Programming for Data Science
</commit_message>
<xml_diff>
--- a/UVA/2--Linear_Models_For_Data_Science/R_Commands.xlsx
+++ b/UVA/2--Linear_Models_For_Data_Science/R_Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlever/Data_Science/Linear_Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Git_Repository\UVA\2--Linear_Models_For_Data_Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DCE3A9-2975-7147-919C-BD73D1CCC903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822B7656-97A8-49E6-B1A8-8D2CE6BF3E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15460" xr2:uid="{4113E9C0-2B3F-A842-BEAE-53D8B59B8F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>R Commands</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>pnorm(q = 0.233, mean = 0, sd = 1, lower.tail = TRUE, log.p = FALSE)</t>
+  </si>
+  <si>
+    <t>Clear console</t>
+  </si>
+  <si>
+    <t>Control + L</t>
   </si>
 </sst>
 </file>
@@ -483,34 +489,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45C9CB9-7864-CD46-9303-21AF865CAB41}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -518,91 +524,99 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>